<commit_message>
Checkpoint work to git
</commit_message>
<xml_diff>
--- a/content/docs/simple_financial_model.xlsx
+++ b/content/docs/simple_financial_model.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27710"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pitosalas/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882042BD-6242-4540-BCB1-4A36922E0A35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="2780" windowWidth="35220" windowHeight="18380" tabRatio="293" activeTab="1"/>
+    <workbookView xWindow="12560" yWindow="3860" windowWidth="38760" windowHeight="20300" tabRatio="293" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Model &quot;Paid Engine&quot;" sheetId="1" r:id="rId1"/>
-    <sheet name="Model &quot;Sticky Engine" sheetId="2" r:id="rId2"/>
+    <sheet name="Simple Model" sheetId="1" r:id="rId1"/>
+    <sheet name="Complicated Model" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
   <si>
     <t>Customers</t>
   </si>
@@ -99,9 +100,6 @@
     <t>Monthly Variable Cost per employee (fully loaded)</t>
   </si>
   <si>
-    <t>Problems with this model</t>
-  </si>
-  <si>
     <t>Current Customers</t>
   </si>
   <si>
@@ -129,9 +127,6 @@
     <t>Fixed Costs</t>
   </si>
   <si>
-    <t>Total Revenue</t>
-  </si>
-  <si>
     <t>Monthly Marketing Costs</t>
   </si>
   <si>
@@ -171,9 +166,6 @@
     <t>Checking Account</t>
   </si>
   <si>
-    <t>Product monthly subscription</t>
-  </si>
-  <si>
     <t>Monthly % growth</t>
   </si>
   <si>
@@ -193,12 +185,18 @@
   </si>
   <si>
     <t>Change in month churn each month</t>
+  </si>
+  <si>
+    <t>Product Price</t>
+  </si>
+  <si>
+    <t>Revenue this month</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
@@ -580,12 +578,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -604,7 +605,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.395550998410581"/>
-          <c:y val="0.0"/>
+          <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -620,7 +621,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Model "Paid Engine"'!$A$10</c:f>
+              <c:f>'Simple Model'!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -634,86 +635,91 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Model "Paid Engine"'!$B$10:$Y$10</c:f>
+              <c:f>'Simple Model'!$B$10:$Y$10</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0_);[Red]\("$"#,##0\)</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>45328.33333333334</c:v>
+                  <c:v>52333.333333333336</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40904.16666666667</c:v>
+                  <c:v>50916.666666666672</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36851.25000000001</c:v>
+                  <c:v>51375.000000000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33243.83333333334</c:v>
+                  <c:v>52958.333333333343</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26093.45000000001</c:v>
+                  <c:v>53075.000000000007</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19597.95166666668</c:v>
+                  <c:v>53664.166666666679</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13953.80383333335</c:v>
+                  <c:v>57230.083333333343</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9416.411650000013</c:v>
+                  <c:v>64665.775000000016</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6317.80181166668</c:v>
+                  <c:v>77132.174166666679</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4466.136672333347</c:v>
+                  <c:v>86691.942333333354</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-55.86149486664999</c:v>
+                  <c:v>95863.664133333354</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-3680.059478786648</c:v>
+                  <c:v>95966.697213333377</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-6316.677261098643</c:v>
+                  <c:v>97430.033601333402</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-8410.125932526236</c:v>
+                  <c:v>92159.868614733423</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-9933.24703752521</c:v>
+                  <c:v>87301.19537880343</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-10857.52419777413</c:v>
+                  <c:v>82874.588481076935</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-11153.0152160355</c:v>
+                  <c:v>78901.651238464125</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-10788.28078520994</c:v>
+                  <c:v>75405.067133720673</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-9730.309632843091</c:v>
+                  <c:v>72408.653823740067</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-7944.439922857904</c:v>
+                  <c:v>69937.419848260412</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-5394.276727373457</c:v>
+                  <c:v>68017.624174006763</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-2041.605372114787</c:v>
+                  <c:v>66676.838716040453</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2153.699550906818</c:v>
+                  <c:v>65944.013985175829</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7233.769720079504</c:v>
+                  <c:v>65849.548017767986</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6F7C-5A4E-B3D4-BED0A5E24CCC}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -767,14 +773,14 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -788,7 +794,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -799,9 +804,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.103740824769785"/>
-          <c:y val="0.134933333333333"/>
-          <c:w val="0.636372169580497"/>
-          <c:h val="0.811644724409449"/>
+          <c:y val="0.13493333333333299"/>
+          <c:w val="0.63637216958049703"/>
+          <c:h val="0.81164472440944901"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -812,7 +817,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Model "Sticky Engine'!$A$19</c:f>
+              <c:f>'Complicated Model'!$A$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -826,86 +831,91 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Model "Sticky Engine'!$B$19:$Y$19</c:f>
+              <c:f>'Complicated Model'!$B$19:$Y$19</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0_);[Red]\("$"#,##0\)</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>150000.0</c:v>
+                  <c:v>150000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>121200.0</c:v>
+                  <c:v>121200</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>95938.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>73829.8809375</c:v>
+                  <c:v>73829.880937499998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54677.55284217773</c:v>
+                  <c:v>54677.552842177734</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38419.52455027811</c:v>
+                  <c:v>38419.524550278118</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25094.01953996541</c:v>
+                  <c:v>25094.019539965408</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14817.74625625217</c:v>
+                  <c:v>14817.746256252169</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7772.328433356666</c:v>
+                  <c:v>7772.3284333566662</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4196.11746817955</c:v>
+                  <c:v>4196.1174681795492</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4379.644519076417</c:v>
+                  <c:v>4379.6445190764171</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8663.605703622012</c:v>
+                  <c:v>8663.6057036220118</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17438.67053524661</c:v>
+                  <c:v>17438.670535246612</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>31146.65543387868</c:v>
+                  <c:v>31146.655433878677</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>50282.76641398878</c:v>
+                  <c:v>50282.766413988778</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>75398.7214076335</c:v>
+                  <c:v>75398.721407633508</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>107106.6336106824</c:v>
+                  <c:v>107106.63361068236</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>146083.5854573999</c:v>
+                  <c:v>146083.58545739989</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>193076.85632573</c:v>
+                  <c:v>193076.85632573004</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>248909.790948335</c:v>
+                  <c:v>248909.79094833502</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>314488.313043337</c:v>
+                  <c:v>314488.31304333702</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>390808.1020367817</c:v>
+                  <c:v>390808.10203678173</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>478962.4613534566</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>580150.9155633064</c:v>
+                  <c:v>580150.91556330642</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7507-C84F-8F06-E43E70804975}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -940,7 +950,7 @@
         <c:axId val="-110472528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="300000.0"/>
+          <c:max val="300000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -960,14 +970,14 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -981,7 +991,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -995,7 +1004,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Model "Sticky Engine'!$A$18</c:f>
+              <c:f>'Complicated Model'!$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1009,86 +1018,91 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Model "Sticky Engine'!$B$18:$Y$18</c:f>
+              <c:f>'Complicated Model'!$B$18:$Y$18</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"_);_(@_)</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>-28800.0</c:v>
+                  <c:v>-28800</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-25261.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-22108.6190625</c:v>
+                  <c:v>-22108.619062499998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-19152.32809532226</c:v>
+                  <c:v>-19152.328095322264</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-16258.02829189962</c:v>
+                  <c:v>-16258.028291899616</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-13325.50501031271</c:v>
+                  <c:v>-13325.505010312711</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-10276.27328371324</c:v>
+                  <c:v>-10276.273283713239</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-7045.417822895502</c:v>
+                  <c:v>-7045.4178228955025</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>-3576.210965177117</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>183.5270508968679</c:v>
+                  <c:v>183.52705089686788</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4283.961184545594</c:v>
+                  <c:v>4283.9611845455947</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8775.064831624601</c:v>
+                  <c:v>8775.0648316246006</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13707.98489863206</c:v>
+                  <c:v>13707.984898632065</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>19136.1109801101</c:v>
+                  <c:v>19136.110980110105</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>25115.95499364474</c:v>
+                  <c:v>25115.954993644737</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>31707.91220304885</c:v>
+                  <c:v>31707.912203048851</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>38976.95184671752</c:v>
+                  <c:v>38976.951846717522</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>46993.27086833013</c:v>
+                  <c:v>46993.270868330132</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>55832.934622605</c:v>
+                  <c:v>55832.934622604997</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>65578.522095002</c:v>
+                  <c:v>65578.522095002001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>76319.7889934447</c:v>
+                  <c:v>76319.788993444701</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>88154.3593166749</c:v>
+                  <c:v>88154.359316674905</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>101188.4542098498</c:v>
+                  <c:v>101188.45420984982</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>115537.6657786386</c:v>
+                  <c:v>115537.66577863859</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6F13-0D4D-8F3E-14AD3C7E6D9A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1123,7 +1137,7 @@
         <c:axId val="-110449152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="100000.0"/>
+          <c:max val="100000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1143,7 +1157,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1153,20 +1167,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1752600</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>254000</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>279400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1201,7 +1221,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1231,7 +1257,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1570,11 +1602,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U21" sqref="U21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V28" sqref="V28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1586,7 +1618,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1620,19 +1652,19 @@
         <v>3</v>
       </c>
       <c r="I2" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="M2" s="26" t="s">
         <v>50</v>
-      </c>
-      <c r="K2" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="L2" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="M2" s="26" t="s">
-        <v>53</v>
       </c>
       <c r="N2" s="25" t="s">
         <v>17</v>
@@ -1656,19 +1688,19 @@
         <v>3</v>
       </c>
       <c r="U2" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="V2" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="W2" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="X2" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="V2" s="25" t="s">
+      <c r="Y2" s="26" t="s">
         <v>50</v>
-      </c>
-      <c r="W2" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="X2" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y2" s="26" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -1773,7 +1805,7 @@
     </row>
     <row r="4" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" s="16">
         <v>0.5</v>
@@ -1850,103 +1882,103 @@
     </row>
     <row r="5" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="B5" s="17">
-        <f t="shared" ref="B5:Y5" si="1">B3*$D$16</f>
-        <v>495</v>
+        <f>B3*D29</f>
+        <v>7500</v>
       </c>
       <c r="C5" s="17">
-        <f t="shared" si="1"/>
-        <v>742.5</v>
+        <f>(C3-B3)*$D$29</f>
+        <v>3750</v>
       </c>
       <c r="D5" s="17">
-        <f t="shared" si="1"/>
-        <v>1113.75</v>
+        <f>(D3-C3)*$D$29</f>
+        <v>5625</v>
       </c>
       <c r="E5" s="17">
-        <f t="shared" si="1"/>
-        <v>1559.25</v>
+        <f>(E3-D3)*$D$29</f>
+        <v>6750</v>
       </c>
       <c r="F5" s="17">
-        <f t="shared" si="1"/>
-        <v>2182.9500000000003</v>
+        <f>(F3-E3)*$D$29</f>
+        <v>9450</v>
       </c>
       <c r="G5" s="17">
-        <f t="shared" si="1"/>
-        <v>2837.8350000000005</v>
+        <f>(G3-F3)*$D$29</f>
+        <v>9922.5000000000055</v>
       </c>
       <c r="H5" s="17">
-        <f t="shared" si="1"/>
-        <v>3689.1855000000005</v>
+        <f>(H3-G3)*$D$29</f>
+        <v>12899.25</v>
       </c>
       <c r="I5" s="17">
-        <f t="shared" si="1"/>
-        <v>4795.9411500000015</v>
+        <f>(I3-H3)*$D$29</f>
+        <v>16769.025000000009</v>
       </c>
       <c r="J5" s="17">
-        <f t="shared" si="1"/>
-        <v>6234.7234950000011</v>
+        <f>(J3-I3)*$D$29</f>
+        <v>21799.732499999998</v>
       </c>
       <c r="K5" s="17">
-        <f t="shared" si="1"/>
-        <v>7481.6681940000017</v>
+        <f>(K3-J3)*$D$29</f>
+        <v>18893.101500000004</v>
       </c>
       <c r="L5" s="17">
-        <f t="shared" si="1"/>
-        <v>8978.0018328000024</v>
-      </c>
-      <c r="M5" s="24">
-        <f t="shared" si="1"/>
-        <v>9875.8020160800024</v>
+        <f>(L3-K3)*$D$29</f>
+        <v>22671.721799999999</v>
+      </c>
+      <c r="M5" s="17">
+        <f>(M3-L3)*$D$29</f>
+        <v>13603.033080000017</v>
       </c>
       <c r="N5" s="17">
-        <f t="shared" si="1"/>
-        <v>10863.382217688004</v>
+        <f>(N3-M3)*$D$29</f>
+        <v>14963.336388000027</v>
       </c>
       <c r="O5" s="17">
-        <f t="shared" si="1"/>
-        <v>11406.551328572406</v>
+        <f>(O3-N3)*$D$29</f>
+        <v>8229.8350134000211</v>
       </c>
       <c r="P5" s="17">
-        <f t="shared" si="1"/>
-        <v>11976.878895001026</v>
+        <f>(P3-O3)*$D$29</f>
+        <v>8641.3267640700033</v>
       </c>
       <c r="Q5" s="17">
-        <f t="shared" si="1"/>
-        <v>12575.722839751077</v>
+        <f>(Q3-P3)*$D$29</f>
+        <v>9073.3931022735087</v>
       </c>
       <c r="R5" s="17">
-        <f t="shared" si="1"/>
-        <v>13204.508981738632</v>
+        <f>(R3-Q3)*$D$29</f>
+        <v>9527.0627573871934</v>
       </c>
       <c r="S5" s="17">
-        <f t="shared" si="1"/>
-        <v>13864.734430825565</v>
+        <f>(S3-R3)*$D$29</f>
+        <v>10003.415895256547</v>
       </c>
       <c r="T5" s="17">
-        <f t="shared" si="1"/>
-        <v>14557.971152366845</v>
+        <f>(T3-S3)*$D$29</f>
+        <v>10503.586690019392</v>
       </c>
       <c r="U5" s="17">
-        <f t="shared" si="1"/>
-        <v>15285.869709985187</v>
+        <f>(U3-T3)*$D$29</f>
+        <v>11028.766024520348</v>
       </c>
       <c r="V5" s="17">
-        <f t="shared" si="1"/>
-        <v>16050.163195484447</v>
+        <f>(V3-U3)*$D$29</f>
+        <v>11580.204325746354</v>
       </c>
       <c r="W5" s="17">
-        <f t="shared" si="1"/>
-        <v>16852.67135525867</v>
+        <f>(W3-V3)*$D$29</f>
+        <v>12159.214542033693</v>
       </c>
       <c r="X5" s="17">
-        <f t="shared" si="1"/>
-        <v>17695.304923021606</v>
-      </c>
-      <c r="Y5" s="24">
-        <f t="shared" si="1"/>
-        <v>18580.070169172686</v>
+        <f>(X3-W3)*$D$29</f>
+        <v>12767.175269135372</v>
+      </c>
+      <c r="Y5" s="17">
+        <f>(Y3-X3)*$D$29</f>
+        <v>13405.534032592152</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
@@ -2031,99 +2063,99 @@
         <v>6</v>
       </c>
       <c r="B7" s="17">
-        <f t="shared" ref="B7:Y7" si="2">B6*$D$18</f>
+        <f>B6*$D$31</f>
         <v>4166.666666666667</v>
       </c>
       <c r="C7" s="17">
-        <f t="shared" si="2"/>
+        <f>C6*$D$31</f>
         <v>4166.666666666667</v>
       </c>
       <c r="D7" s="17">
-        <f t="shared" si="2"/>
+        <f>D6*$D$31</f>
         <v>4166.666666666667</v>
       </c>
       <c r="E7" s="17">
-        <f t="shared" si="2"/>
+        <f>E6*$D$31</f>
         <v>4166.666666666667</v>
       </c>
       <c r="F7" s="17">
-        <f t="shared" si="2"/>
+        <f>F6*$D$31</f>
         <v>8333.3333333333339</v>
       </c>
       <c r="G7" s="17">
-        <f t="shared" si="2"/>
+        <f>G6*$D$31</f>
         <v>8333.3333333333339</v>
       </c>
       <c r="H7" s="17">
-        <f t="shared" si="2"/>
+        <f>H6*$D$31</f>
         <v>8333.3333333333339</v>
       </c>
       <c r="I7" s="17">
-        <f t="shared" si="2"/>
+        <f>I6*$D$31</f>
         <v>8333.3333333333339</v>
       </c>
       <c r="J7" s="17">
-        <f t="shared" si="2"/>
+        <f>J6*$D$31</f>
         <v>8333.3333333333339</v>
       </c>
       <c r="K7" s="17">
-        <f t="shared" si="2"/>
+        <f>K6*$D$31</f>
         <v>8333.3333333333339</v>
       </c>
       <c r="L7" s="17">
-        <f t="shared" si="2"/>
+        <f>L6*$D$31</f>
         <v>12500</v>
       </c>
       <c r="M7" s="24">
-        <f t="shared" si="2"/>
+        <f>M6*$D$31</f>
         <v>12500</v>
       </c>
       <c r="N7" s="17">
-        <f t="shared" si="2"/>
+        <f>N6*$D$31</f>
         <v>12500</v>
       </c>
       <c r="O7" s="17">
-        <f t="shared" si="2"/>
+        <f>O6*$D$31</f>
         <v>12500</v>
       </c>
       <c r="P7" s="17">
-        <f t="shared" si="2"/>
+        <f>P6*$D$31</f>
         <v>12500</v>
       </c>
       <c r="Q7" s="17">
-        <f t="shared" si="2"/>
+        <f>Q6*$D$31</f>
         <v>12500</v>
       </c>
       <c r="R7" s="17">
-        <f t="shared" si="2"/>
+        <f>R6*$D$31</f>
         <v>12500</v>
       </c>
       <c r="S7" s="17">
-        <f t="shared" si="2"/>
+        <f>S6*$D$31</f>
         <v>12500</v>
       </c>
       <c r="T7" s="17">
-        <f t="shared" si="2"/>
+        <f>T6*$D$31</f>
         <v>12500</v>
       </c>
       <c r="U7" s="17">
-        <f t="shared" si="2"/>
+        <f>U6*$D$31</f>
         <v>12500</v>
       </c>
       <c r="V7" s="17">
-        <f t="shared" si="2"/>
+        <f>V6*$D$31</f>
         <v>12500</v>
       </c>
       <c r="W7" s="17">
-        <f t="shared" si="2"/>
+        <f>W6*$D$31</f>
         <v>12500</v>
       </c>
       <c r="X7" s="17">
-        <f t="shared" si="2"/>
+        <f>X6*$D$31</f>
         <v>12500</v>
       </c>
       <c r="Y7" s="24">
-        <f t="shared" si="2"/>
+        <f>Y6*$D$31</f>
         <v>12500</v>
       </c>
     </row>
@@ -2132,99 +2164,99 @@
         <v>8</v>
       </c>
       <c r="B8" s="17">
-        <f t="shared" ref="B8:Y8" si="3">B7+$D$19</f>
+        <f>B7+$D$32</f>
         <v>5166.666666666667</v>
       </c>
       <c r="C8" s="17">
-        <f t="shared" si="3"/>
+        <f>C7+$D$32</f>
         <v>5166.666666666667</v>
       </c>
       <c r="D8" s="17">
-        <f t="shared" si="3"/>
+        <f>D7+$D$32</f>
         <v>5166.666666666667</v>
       </c>
       <c r="E8" s="17">
-        <f t="shared" si="3"/>
+        <f>E7+$D$32</f>
         <v>5166.666666666667</v>
       </c>
       <c r="F8" s="17">
-        <f t="shared" si="3"/>
+        <f>F7+$D$32</f>
         <v>9333.3333333333339</v>
       </c>
       <c r="G8" s="17">
-        <f t="shared" si="3"/>
+        <f>G7+$D$32</f>
         <v>9333.3333333333339</v>
       </c>
       <c r="H8" s="17">
-        <f t="shared" si="3"/>
+        <f>H7+$D$32</f>
         <v>9333.3333333333339</v>
       </c>
       <c r="I8" s="17">
-        <f t="shared" si="3"/>
+        <f>I7+$D$32</f>
         <v>9333.3333333333339</v>
       </c>
       <c r="J8" s="17">
-        <f t="shared" si="3"/>
+        <f>J7+$D$32</f>
         <v>9333.3333333333339</v>
       </c>
       <c r="K8" s="17">
-        <f t="shared" si="3"/>
+        <f>K7+$D$32</f>
         <v>9333.3333333333339</v>
       </c>
       <c r="L8" s="17">
-        <f t="shared" si="3"/>
+        <f>L7+$D$32</f>
         <v>13500</v>
       </c>
       <c r="M8" s="24">
-        <f t="shared" si="3"/>
+        <f>M7+$D$32</f>
         <v>13500</v>
       </c>
       <c r="N8" s="17">
-        <f t="shared" si="3"/>
+        <f>N7+$D$32</f>
         <v>13500</v>
       </c>
       <c r="O8" s="17">
-        <f t="shared" si="3"/>
+        <f>O7+$D$32</f>
         <v>13500</v>
       </c>
       <c r="P8" s="17">
-        <f t="shared" si="3"/>
+        <f>P7+$D$32</f>
         <v>13500</v>
       </c>
       <c r="Q8" s="17">
-        <f t="shared" si="3"/>
+        <f>Q7+$D$32</f>
         <v>13500</v>
       </c>
       <c r="R8" s="17">
-        <f t="shared" si="3"/>
+        <f>R7+$D$32</f>
         <v>13500</v>
       </c>
       <c r="S8" s="17">
-        <f t="shared" si="3"/>
+        <f>S7+$D$32</f>
         <v>13500</v>
       </c>
       <c r="T8" s="17">
-        <f t="shared" si="3"/>
+        <f>T7+$D$32</f>
         <v>13500</v>
       </c>
       <c r="U8" s="17">
-        <f t="shared" si="3"/>
+        <f>U7+$D$32</f>
         <v>13500</v>
       </c>
       <c r="V8" s="17">
-        <f t="shared" si="3"/>
+        <f>V7+$D$32</f>
         <v>13500</v>
       </c>
       <c r="W8" s="17">
-        <f t="shared" si="3"/>
+        <f>W7+$D$32</f>
         <v>13500</v>
       </c>
       <c r="X8" s="17">
-        <f t="shared" si="3"/>
+        <f>X7+$D$32</f>
         <v>13500</v>
       </c>
       <c r="Y8" s="24">
-        <f t="shared" si="3"/>
+        <f>Y7+$D$32</f>
         <v>13500</v>
       </c>
     </row>
@@ -2234,200 +2266,200 @@
       </c>
       <c r="B9" s="17">
         <f>B5-B8</f>
-        <v>-4671.666666666667</v>
+        <v>2333.333333333333</v>
       </c>
       <c r="C9" s="17">
-        <f t="shared" ref="C9:H9" si="4">C5-C8</f>
-        <v>-4424.166666666667</v>
+        <f t="shared" ref="C9:H9" si="1">C5-C8</f>
+        <v>-1416.666666666667</v>
       </c>
       <c r="D9" s="17">
-        <f t="shared" si="4"/>
-        <v>-4052.916666666667</v>
+        <f t="shared" si="1"/>
+        <v>458.33333333333303</v>
       </c>
       <c r="E9" s="17">
-        <f t="shared" si="4"/>
-        <v>-3607.416666666667</v>
+        <f t="shared" si="1"/>
+        <v>1583.333333333333</v>
       </c>
       <c r="F9" s="17">
-        <f t="shared" si="4"/>
-        <v>-7150.3833333333332</v>
+        <f t="shared" si="1"/>
+        <v>116.66666666666606</v>
       </c>
       <c r="G9" s="17">
-        <f t="shared" si="4"/>
-        <v>-6495.498333333333</v>
+        <f t="shared" si="1"/>
+        <v>589.16666666667152</v>
       </c>
       <c r="H9" s="17">
-        <f t="shared" si="4"/>
-        <v>-5644.1478333333334</v>
+        <f t="shared" si="1"/>
+        <v>3565.9166666666661</v>
       </c>
       <c r="I9" s="17">
-        <f t="shared" ref="I9" si="5">I5-I8</f>
-        <v>-4537.3921833333325</v>
+        <f t="shared" ref="I9" si="2">I5-I8</f>
+        <v>7435.6916666666748</v>
       </c>
       <c r="J9" s="17">
-        <f t="shared" ref="J9" si="6">J5-J8</f>
-        <v>-3098.6098383333328</v>
+        <f t="shared" ref="J9" si="3">J5-J8</f>
+        <v>12466.399166666664</v>
       </c>
       <c r="K9" s="17">
-        <f t="shared" ref="K9" si="7">K5-K8</f>
-        <v>-1851.6651393333323</v>
+        <f t="shared" ref="K9" si="4">K5-K8</f>
+        <v>9559.7681666666704</v>
       </c>
       <c r="L9" s="17">
-        <f t="shared" ref="L9" si="8">L5-L8</f>
-        <v>-4521.9981671999976</v>
+        <f t="shared" ref="L9" si="5">L5-L8</f>
+        <v>9171.7217999999993</v>
       </c>
       <c r="M9" s="24">
-        <f t="shared" ref="M9:N9" si="9">M5-M8</f>
-        <v>-3624.1979839199976</v>
+        <f t="shared" ref="M9:N9" si="6">M5-M8</f>
+        <v>103.03308000001743</v>
       </c>
       <c r="N9" s="17">
-        <f t="shared" si="9"/>
-        <v>-2636.6177823119961</v>
+        <f t="shared" si="6"/>
+        <v>1463.336388000027</v>
       </c>
       <c r="O9" s="17">
-        <f t="shared" ref="O9" si="10">O5-O8</f>
-        <v>-2093.4486714275936</v>
+        <f t="shared" ref="O9" si="7">O5-O8</f>
+        <v>-5270.1649865999789</v>
       </c>
       <c r="P9" s="17">
-        <f t="shared" ref="P9" si="11">P5-P8</f>
-        <v>-1523.1211049989743</v>
+        <f t="shared" ref="P9" si="8">P5-P8</f>
+        <v>-4858.6732359299967</v>
       </c>
       <c r="Q9" s="17">
-        <f t="shared" ref="Q9" si="12">Q5-Q8</f>
-        <v>-924.27716024892288</v>
+        <f t="shared" ref="Q9" si="9">Q5-Q8</f>
+        <v>-4426.6068977264913</v>
       </c>
       <c r="R9" s="17">
-        <f t="shared" ref="R9" si="13">R5-R8</f>
-        <v>-295.49101826136757</v>
+        <f t="shared" ref="R9" si="10">R5-R8</f>
+        <v>-3972.9372426128066</v>
       </c>
       <c r="S9" s="17">
-        <f t="shared" ref="S9" si="14">S5-S8</f>
-        <v>364.73443082556514</v>
+        <f t="shared" ref="S9" si="11">S5-S8</f>
+        <v>-3496.5841047434533</v>
       </c>
       <c r="T9" s="17">
-        <f t="shared" ref="T9" si="15">T5-T8</f>
-        <v>1057.9711523668448</v>
+        <f t="shared" ref="T9" si="12">T5-T8</f>
+        <v>-2996.4133099806077</v>
       </c>
       <c r="U9" s="17">
-        <f t="shared" ref="U9" si="16">U5-U8</f>
-        <v>1785.869709985187</v>
+        <f t="shared" ref="U9" si="13">U5-U8</f>
+        <v>-2471.2339754796521</v>
       </c>
       <c r="V9" s="17">
-        <f t="shared" ref="V9" si="17">V5-V8</f>
-        <v>2550.163195484447</v>
+        <f t="shared" ref="V9" si="14">V5-V8</f>
+        <v>-1919.7956742536462</v>
       </c>
       <c r="W9" s="17">
-        <f t="shared" ref="W9" si="18">W5-W8</f>
-        <v>3352.6713552586698</v>
+        <f t="shared" ref="W9" si="15">W5-W8</f>
+        <v>-1340.7854579663071</v>
       </c>
       <c r="X9" s="17">
-        <f t="shared" ref="X9" si="19">X5-X8</f>
-        <v>4195.3049230216056</v>
+        <f t="shared" ref="X9" si="16">X5-X8</f>
+        <v>-732.82473086462778</v>
       </c>
       <c r="Y9" s="24">
-        <f t="shared" ref="Y9" si="20">Y5-Y8</f>
-        <v>5080.0701691726863</v>
+        <f t="shared" ref="Y9" si="17">Y5-Y8</f>
+        <v>-94.465967407848439</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="17">
-        <f>D20+B9</f>
-        <v>45328.333333333336</v>
+        <f>D33+B9</f>
+        <v>52333.333333333336</v>
       </c>
       <c r="C10" s="17">
         <f>B10+C9</f>
-        <v>40904.166666666672</v>
+        <v>50916.666666666672</v>
       </c>
       <c r="D10" s="17">
-        <f t="shared" ref="D10:H10" si="21">C10+D9</f>
-        <v>36851.250000000007</v>
+        <f t="shared" ref="D10:H10" si="18">C10+D9</f>
+        <v>51375.000000000007</v>
       </c>
       <c r="E10" s="17">
-        <f t="shared" si="21"/>
-        <v>33243.833333333343</v>
+        <f t="shared" si="18"/>
+        <v>52958.333333333343</v>
       </c>
       <c r="F10" s="17">
-        <f t="shared" si="21"/>
-        <v>26093.450000000012</v>
+        <f t="shared" si="18"/>
+        <v>53075.000000000007</v>
       </c>
       <c r="G10" s="17">
-        <f t="shared" si="21"/>
-        <v>19597.951666666679</v>
+        <f t="shared" si="18"/>
+        <v>53664.166666666679</v>
       </c>
       <c r="H10" s="17">
-        <f t="shared" si="21"/>
-        <v>13953.803833333346</v>
+        <f t="shared" si="18"/>
+        <v>57230.083333333343</v>
       </c>
       <c r="I10" s="17">
-        <f t="shared" ref="I10" si="22">H10+I9</f>
-        <v>9416.4116500000127</v>
+        <f t="shared" ref="I10" si="19">H10+I9</f>
+        <v>64665.775000000016</v>
       </c>
       <c r="J10" s="17">
-        <f t="shared" ref="J10" si="23">I10+J9</f>
-        <v>6317.8018116666799</v>
+        <f t="shared" ref="J10" si="20">I10+J9</f>
+        <v>77132.174166666679</v>
       </c>
       <c r="K10" s="17">
-        <f t="shared" ref="K10" si="24">J10+K9</f>
-        <v>4466.1366723333476</v>
+        <f t="shared" ref="K10" si="21">J10+K9</f>
+        <v>86691.942333333354</v>
       </c>
       <c r="L10" s="17">
-        <f t="shared" ref="L10" si="25">K10+L9</f>
-        <v>-55.861494866649991</v>
+        <f t="shared" ref="L10" si="22">K10+L9</f>
+        <v>95863.664133333354</v>
       </c>
       <c r="M10" s="24">
-        <f t="shared" ref="M10:N10" si="26">L10+M9</f>
-        <v>-3680.0594787866476</v>
+        <f t="shared" ref="M10:N10" si="23">L10+M9</f>
+        <v>95966.697213333377</v>
       </c>
       <c r="N10" s="17">
-        <f t="shared" si="26"/>
-        <v>-6316.6772610986436</v>
+        <f t="shared" si="23"/>
+        <v>97430.033601333402</v>
       </c>
       <c r="O10" s="17">
         <f>N10+O9</f>
-        <v>-8410.1259325262363</v>
+        <v>92159.868614733423</v>
       </c>
       <c r="P10" s="17">
-        <f t="shared" ref="P10" si="27">O10+P9</f>
-        <v>-9933.2470375252105</v>
+        <f t="shared" ref="P10" si="24">O10+P9</f>
+        <v>87301.19537880343</v>
       </c>
       <c r="Q10" s="17">
-        <f t="shared" ref="Q10" si="28">P10+Q9</f>
-        <v>-10857.524197774133</v>
+        <f t="shared" ref="Q10" si="25">P10+Q9</f>
+        <v>82874.588481076935</v>
       </c>
       <c r="R10" s="17">
-        <f t="shared" ref="R10" si="29">Q10+R9</f>
-        <v>-11153.015216035501</v>
+        <f t="shared" ref="R10" si="26">Q10+R9</f>
+        <v>78901.651238464125</v>
       </c>
       <c r="S10" s="17">
-        <f t="shared" ref="S10" si="30">R10+S9</f>
-        <v>-10788.280785209936</v>
+        <f t="shared" ref="S10" si="27">R10+S9</f>
+        <v>75405.067133720673</v>
       </c>
       <c r="T10" s="17">
-        <f t="shared" ref="T10" si="31">S10+T9</f>
-        <v>-9730.3096328430911</v>
+        <f t="shared" ref="T10" si="28">S10+T9</f>
+        <v>72408.653823740067</v>
       </c>
       <c r="U10" s="17">
-        <f t="shared" ref="U10" si="32">T10+U9</f>
-        <v>-7944.4399228579041</v>
+        <f t="shared" ref="U10" si="29">T10+U9</f>
+        <v>69937.419848260412</v>
       </c>
       <c r="V10" s="17">
-        <f t="shared" ref="V10" si="33">U10+V9</f>
-        <v>-5394.2767273734571</v>
+        <f t="shared" ref="V10" si="30">U10+V9</f>
+        <v>68017.624174006763</v>
       </c>
       <c r="W10" s="17">
-        <f t="shared" ref="W10" si="34">V10+W9</f>
-        <v>-2041.6053721147873</v>
+        <f t="shared" ref="W10" si="31">V10+W9</f>
+        <v>66676.838716040453</v>
       </c>
       <c r="X10" s="17">
-        <f t="shared" ref="X10" si="35">W10+X9</f>
-        <v>2153.6995509068183</v>
+        <f t="shared" ref="X10" si="32">W10+X9</f>
+        <v>65944.013985175829</v>
       </c>
       <c r="Y10" s="24">
-        <f t="shared" ref="Y10" si="36">X10+Y9</f>
-        <v>7233.7697200795046</v>
+        <f t="shared" ref="Y10" si="33">X10+Y9</f>
+        <v>65849.548017767986</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2436,71 +2468,69 @@
     <row r="14" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" s="16"/>
     </row>
-    <row r="15" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="18">
-        <v>4.95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="17">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="17">
-        <f>D17/12</f>
-        <v>4166.666666666667</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="17">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="17">
-        <v>50000</v>
-      </c>
-    </row>
+    <row r="15" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19" t="s">
-        <v>23</v>
-      </c>
+      <c r="A22" s="19"/>
     </row>
     <row r="23" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="18">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="17">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="17">
+        <f>D30/12</f>
+        <v>4166.666666666667</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="17">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="17">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:4" ht="23" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2509,10 +2539,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -2524,7 +2554,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2537,7 +2567,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
@@ -2614,7 +2644,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="6">
         <v>0.25</v>
@@ -2714,7 +2744,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <f>1/B4</f>
@@ -2822,7 +2852,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="4">
         <v>0</v>
@@ -2922,7 +2952,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -3022,7 +3052,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>140</v>
@@ -3223,7 +3253,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="7">
         <f>B10*$B$31</f>
@@ -3324,7 +3354,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B14" s="10">
         <f>$B$32</f>
@@ -3425,7 +3455,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="8">
         <f>$B$33</f>
@@ -3627,7 +3657,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B18" s="7">
         <f>B12-B16</f>
@@ -3728,7 +3758,7 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B19" s="5">
         <f>$B$34</f>
@@ -3855,7 +3885,7 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B21" s="5">
         <f>B16/B10</f>
@@ -3956,7 +3986,7 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B22" s="5">
         <f>B14/B9</f>
@@ -4055,9 +4085,9 @@
         <v>4.8661509797263509</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B23" s="5">
         <f>$B$31*B5</f>
@@ -4219,7 +4249,7 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="6">
         <v>0.08</v>
@@ -4227,7 +4257,7 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="5">
         <v>30</v>
@@ -4235,7 +4265,7 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B32" s="5">
         <v>4000</v>
@@ -4243,7 +4273,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B33">
         <v>29000</v>
@@ -4259,7 +4289,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B35" s="27">
         <v>-0.05</v>
@@ -4267,12 +4297,12 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A43" r:id="rId1" location="gid=0"/>
+    <hyperlink ref="A43" r:id="rId1" location="gid=0" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>